<commit_message>
Re-test the UI automation script for all the modules
</commit_message>
<xml_diff>
--- a/tests/artifact/data/BalanceSheet.data.xlsx
+++ b/tests/artifact/data/BalanceSheet.data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="9215" tabRatio="500"/>
+    <workbookView windowWidth="18350" windowHeight="6950" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="#default" sheetId="2" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="207">
   <si>
     <t>login.screen</t>
   </si>
@@ -184,7 +184,7 @@
     <t>org.open</t>
   </si>
   <si>
-    <t>//button[text()=' Open ']</t>
+    <t>(//button[text()=' Open '])[2]</t>
   </si>
   <si>
     <t>org.hamburger</t>
@@ -376,7 +376,7 @@
     <t>calender.from</t>
   </si>
   <si>
-    <t>(//button[@aria-haspopup='dialog'])[1]</t>
+    <t>(//*[@aria-haspopup='dialog'])[1]</t>
   </si>
   <si>
     <t>label.To</t>
@@ -388,7 +388,7 @@
     <t>calender.To</t>
   </si>
   <si>
-    <t>(//button[@aria-haspopup='dialog'])[2]</t>
+    <t>(//*[@aria-haspopup='dialog'])[2]</t>
   </si>
   <si>
     <t>button.getdetails</t>
@@ -463,145 +463,67 @@
     <t>label.liab</t>
   </si>
   <si>
-    <t>//span[contains(text(),'Capital and Liabilities')]</t>
+    <t>//*[contains(text(),'Capital and Liabilities')]</t>
   </si>
   <si>
     <t>label.capital</t>
   </si>
   <si>
-    <t>//button[text()=' Capital ']</t>
+    <t>//*[text()=' Capital ']</t>
   </si>
   <si>
     <t>label.loanlib</t>
   </si>
   <si>
-    <t>//button[text()=' Loans(Liability) ']</t>
+    <t>//*[text()=' Loans(Liability) ']</t>
   </si>
   <si>
     <t>label.currentlib</t>
   </si>
   <si>
-    <t>//button[text()=' Current Liabilities ']</t>
+    <t>//*[text()=' Current Liabilities ']</t>
   </si>
   <si>
     <t>label.reserves</t>
   </si>
   <si>
-    <t>//button[text()=' Reserves ']</t>
-  </si>
-  <si>
-    <t>label.capital.amount</t>
-  </si>
-  <si>
-    <t>(//span[text()=' 75000000.00 '])[1]</t>
-  </si>
-  <si>
-    <t>label.loanlib.amount</t>
-  </si>
-  <si>
-    <t>//span[text()=' 1800000.00 ']</t>
-  </si>
-  <si>
-    <t>label.currentlib.amount</t>
-  </si>
-  <si>
-    <t>(//span[text()=' -187700.00 '])[1]</t>
-  </si>
-  <si>
-    <t>label.reserves.amount</t>
-  </si>
-  <si>
-    <t>(//span[text()=' 1337613.00 '])[1]</t>
-  </si>
-  <si>
-    <t>label.totalasset.amount</t>
-  </si>
-  <si>
-    <t>(//span[text()=' 77949913.00 '])[1]</t>
+    <t>//*[text()=' Reserves ']</t>
   </si>
   <si>
     <t>label.propnasset</t>
   </si>
   <si>
-    <t>//span[contains(text(),'Property and Assets')]</t>
+    <t>//*[contains(text(),'Property and Assets')]</t>
   </si>
   <si>
     <t>label.fixed</t>
   </si>
   <si>
-    <t>//button[text()=' Fixed Assets ']</t>
+    <t>//*[text()=' Fixed Assets ']</t>
   </si>
   <si>
     <t>label.investments</t>
   </si>
   <si>
-    <t>//button[text()=' Investments ']</t>
+    <t>//*[text()=' Investments ']</t>
   </si>
   <si>
     <t>label.currentassets</t>
   </si>
   <si>
-    <t>//button[text()=' Current Assets ']</t>
+    <t>//*[text()=' Current Assets ']</t>
   </si>
   <si>
     <t>label.loanasset</t>
   </si>
   <si>
-    <t>//button[text()=' Loans(Asset) ']</t>
+    <t>//*[text()=' Loans(Asset) ']</t>
   </si>
   <si>
     <t>label.assetmiscellaneous</t>
   </si>
   <si>
-    <t>//span[text()=' Miscellaneous Expenses(Asset) ']</t>
-  </si>
-  <si>
-    <t>label.fixed.amount</t>
-  </si>
-  <si>
-    <t>//span[text()=' 7750000.00 ']</t>
-  </si>
-  <si>
-    <t>label.investments.amount</t>
-  </si>
-  <si>
-    <t>//span[text()=' 27000.00 ']</t>
-  </si>
-  <si>
-    <t>label.currentassets.amount</t>
-  </si>
-  <si>
-    <t>//span[text()=' 1519913.00 ']</t>
-  </si>
-  <si>
-    <t>label.loanasset.amount</t>
-  </si>
-  <si>
-    <t>//span[text()=' 150000.00 ']</t>
-  </si>
-  <si>
-    <t>label.assetmisc.amount</t>
-  </si>
-  <si>
-    <t>(//span[text()=' 0.00 '])[8]</t>
-  </si>
-  <si>
-    <t>label.totalliab.amount</t>
-  </si>
-  <si>
-    <t>//span[text()=' 9446913.00 ']</t>
-  </si>
-  <si>
-    <t>label.difference.amount</t>
-  </si>
-  <si>
-    <t>//span[text()=' 68503000.00 ']</t>
-  </si>
-  <si>
-    <t>label.gorsstotalasst.amount</t>
-  </si>
-  <si>
-    <t>(//span[text()=' 77949913.00 '])[2]</t>
+    <t>//*[text()=' Miscellaneous Expenses(Asset) ']</t>
   </si>
   <si>
     <t>label.totalasset</t>
@@ -640,52 +562,18 @@
     <t>//span[contains(text(),'31')]</t>
   </si>
   <si>
-    <t>capital.amount</t>
-  </si>
-  <si>
-    <t>//body[1]/div[1]/main[1]/section[1]/div[1]/div[3]/div[1]/div[1]/table[1]/tbody[1]/tr[1]/td[4]/span[1]</t>
-  </si>
-  <si>
-    <t>loanlib.amount</t>
-  </si>
-  <si>
-    <t>//body[1]/div[1]/main[1]/section[1]/div[1]/div[3]/div[1]/div[1]/table[1]/tbody[1]/tr[3]/td[4]</t>
-  </si>
-  <si>
-    <t>currentlib.amount</t>
-  </si>
-  <si>
-    <t>//body[1]/div[1]/main[1]/section[1]/div[1]/div[3]/div[1]/div[1]/table[1]/tbody[1]/tr[6]/td[4]</t>
-  </si>
-  <si>
-    <t>reserves.amount</t>
-  </si>
-  <si>
-    <t>//body[1]/div[1]/main[1]/section[1]/div[1]/div[3]/div[1]/div[1]/table[1]/tbody[1]/tr[11]/td[4]</t>
-  </si>
-  <si>
-    <t>totalliab.amount</t>
-  </si>
-  <si>
-    <t>//body[1]/div[1]/main[1]/section[1]/div[1]/div[3]/div[1]/div[1]/table[1]/tbody[1]/tr[15]/td[4]</t>
-  </si>
-  <si>
-    <t>fixed.amount</t>
-  </si>
-  <si>
-    <t>//body[1]/div[1]/main[1]/section[1]/div[1]/div[3]/div[2]/div[1]/table[1]/tbody[1]/tr[1]/td[4]</t>
-  </si>
-  <si>
-    <t>investments.amount</t>
-  </si>
-  <si>
-    <t>//body[1]/div[1]/main[1]/section[1]/div[1]/div[3]/div[2]/div[1]/table[1]/tbody[1]/tr[7]/td[4]</t>
-  </si>
-  <si>
-    <t>currentasst.amount</t>
-  </si>
-  <si>
-    <t>//body[1]/div[1]/main[1]/section[1]/div[1]/div[3]/div[2]/div[1]/table[1]/tbody[1]/tr[10]/td[4]</t>
+    <t>Capital amount</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Courier New"/>
+        <charset val="134"/>
+      </rPr>
+      <t>//div[@class='col-md-6 col-12'][1]/div/table/thead/tr</t>
+    </r>
   </si>
   <si>
     <t>loanasset.amount</t>
@@ -716,17 +604,77 @@
   </si>
   <si>
     <t>//tbody/tr[21]/td[4]</t>
+  </si>
+  <si>
+    <t>Capital.first.row</t>
+  </si>
+  <si>
+    <t>//div[@class='col-md-6 col-12'][1]/div/table/tbody/tr[@class='bs-row']/td[1]</t>
+  </si>
+  <si>
+    <t>Capital.second.row</t>
+  </si>
+  <si>
+    <t>//div[@class='col-md-6 col-12'][1]/div/table/tbody/tr[@class='bs-row']/td[2]</t>
+  </si>
+  <si>
+    <t>Capital.third.row</t>
+  </si>
+  <si>
+    <t>//div[@class='col-md-6 col-12'][1]/div/table/tbody/tr[@class='bs-row']/td[3]</t>
+  </si>
+  <si>
+    <t>Capital.fourth.row</t>
+  </si>
+  <si>
+    <t>//div[@class='col-md-6 col-12'][1]/div/table/tbody/tr[@class='bs-row']/td[4]</t>
+  </si>
+  <si>
+    <t>Capital and Liabilities</t>
+  </si>
+  <si>
+    <t>//div[@class='col-md-6 col-12'][1]/div/table/tbody/tr[@class='bs-row']</t>
+  </si>
+  <si>
+    <t>Property.first.row</t>
+  </si>
+  <si>
+    <t>//div[@class='col-md-6 col-12'][2]/div/table/tbody/tr[@class='bs-row']/td[1]</t>
+  </si>
+  <si>
+    <t>Property.second.row</t>
+  </si>
+  <si>
+    <t>//div[@class='col-md-6 col-12'][2]/div/table/tbody/tr[@class='bs-row']/td[2]</t>
+  </si>
+  <si>
+    <t>Property.third.row</t>
+  </si>
+  <si>
+    <t>//div[@class='col-md-6 col-12'][2]/div/table/tbody/tr[@class='bs-row']/td[3]</t>
+  </si>
+  <si>
+    <t>Property.fourth.row</t>
+  </si>
+  <si>
+    <t>//div[@class='col-md-6 col-12'][2]/div/table/tbody/tr[@class='bs-row']/td[4]</t>
+  </si>
+  <si>
+    <t>Property and Assets</t>
+  </si>
+  <si>
+    <t>//div[@class='col-md-6 col-12'][2]/div/table/tbody/tr[@class='bs-row']</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="178" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="179" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="27">
     <font>
@@ -787,64 +735,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -880,31 +775,18 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -922,6 +804,72 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -932,19 +880,145 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -956,151 +1030,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1142,6 +1090,39 @@
     </border>
     <border>
       <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
@@ -1152,6 +1133,21 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1173,6 +1169,15 @@
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -1181,210 +1186,153 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="176" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="21" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="6" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1422,52 +1370,52 @@
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
-    <cellStyle name="Comma" xfId="2" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
-    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
-    <cellStyle name="Currency" xfId="5" builtinId="4"/>
-    <cellStyle name="Percent" xfId="6" builtinId="5"/>
-    <cellStyle name="Hyperlink" xfId="7" builtinId="8"/>
-    <cellStyle name="60% - Accent4" xfId="8" builtinId="44"/>
-    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9"/>
-    <cellStyle name="Check Cell" xfId="10" builtinId="23"/>
-    <cellStyle name="Heading 2" xfId="11" builtinId="17"/>
-    <cellStyle name="Note" xfId="12" builtinId="10"/>
-    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
-    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
-    <cellStyle name="Title" xfId="16" builtinId="15"/>
-    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
-    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
-    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
-    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
-    <cellStyle name="Input" xfId="21" builtinId="20"/>
-    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
-    <cellStyle name="Good" xfId="23" builtinId="26"/>
-    <cellStyle name="Output" xfId="24" builtinId="21"/>
-    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
-    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
-    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
-    <cellStyle name="Total" xfId="28" builtinId="25"/>
-    <cellStyle name="Bad" xfId="29" builtinId="27"/>
-    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
-    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
-    <cellStyle name="20% - Accent5" xfId="32" builtinId="46"/>
-    <cellStyle name="60% - Accent1" xfId="33" builtinId="32"/>
-    <cellStyle name="Accent2" xfId="34" builtinId="33"/>
-    <cellStyle name="20% - Accent2" xfId="35" builtinId="34"/>
-    <cellStyle name="20% - Accent6" xfId="36" builtinId="50"/>
-    <cellStyle name="60% - Accent2" xfId="37" builtinId="36"/>
-    <cellStyle name="Accent3" xfId="38" builtinId="37"/>
-    <cellStyle name="20% - Accent3" xfId="39" builtinId="38"/>
-    <cellStyle name="Accent4" xfId="40" builtinId="41"/>
-    <cellStyle name="20% - Accent4" xfId="41" builtinId="42"/>
-    <cellStyle name="40% - Accent4" xfId="42" builtinId="43"/>
-    <cellStyle name="Accent5" xfId="43" builtinId="45"/>
-    <cellStyle name="40% - Accent5" xfId="44" builtinId="47"/>
-    <cellStyle name="60% - Accent5" xfId="45" builtinId="48"/>
-    <cellStyle name="Accent6" xfId="46" builtinId="49"/>
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Currency" xfId="2" builtinId="4"/>
+    <cellStyle name="Percent" xfId="3" builtinId="5"/>
+    <cellStyle name="Comma [0]" xfId="4" builtinId="6"/>
+    <cellStyle name="Currency [0]" xfId="5" builtinId="7"/>
+    <cellStyle name="Hyperlink" xfId="6" builtinId="8"/>
+    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9"/>
+    <cellStyle name="Note" xfId="8" builtinId="10"/>
+    <cellStyle name="Warning Text" xfId="9" builtinId="11"/>
+    <cellStyle name="Title" xfId="10" builtinId="15"/>
+    <cellStyle name="CExplanatory Text" xfId="11" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="12" builtinId="16"/>
+    <cellStyle name="Heading 2" xfId="13" builtinId="17"/>
+    <cellStyle name="Heading 3" xfId="14" builtinId="18"/>
+    <cellStyle name="Heading 4" xfId="15" builtinId="19"/>
+    <cellStyle name="Input" xfId="16" builtinId="20"/>
+    <cellStyle name="Output" xfId="17" builtinId="21"/>
+    <cellStyle name="Calculation" xfId="18" builtinId="22"/>
+    <cellStyle name="Check Cell" xfId="19" builtinId="23"/>
+    <cellStyle name="Linked Cell" xfId="20" builtinId="24"/>
+    <cellStyle name="Total" xfId="21" builtinId="25"/>
+    <cellStyle name="Good" xfId="22" builtinId="26"/>
+    <cellStyle name="Bad" xfId="23" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="24" builtinId="28"/>
+    <cellStyle name="Accent1" xfId="25" builtinId="29"/>
+    <cellStyle name="20% - Accent1" xfId="26" builtinId="30"/>
+    <cellStyle name="40% - Accent1" xfId="27" builtinId="31"/>
+    <cellStyle name="60% - Accent1" xfId="28" builtinId="32"/>
+    <cellStyle name="Accent2" xfId="29" builtinId="33"/>
+    <cellStyle name="20% - Accent2" xfId="30" builtinId="34"/>
+    <cellStyle name="40% - Accent2" xfId="31" builtinId="35"/>
+    <cellStyle name="60% - Accent2" xfId="32" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="33" builtinId="37"/>
+    <cellStyle name="20% - Accent3" xfId="34" builtinId="38"/>
+    <cellStyle name="40% - Accent3" xfId="35" builtinId="39"/>
+    <cellStyle name="60% - Accent3" xfId="36" builtinId="40"/>
+    <cellStyle name="Accent4" xfId="37" builtinId="41"/>
+    <cellStyle name="20% - Accent4" xfId="38" builtinId="42"/>
+    <cellStyle name="40% - Accent4" xfId="39" builtinId="43"/>
+    <cellStyle name="60% - Accent4" xfId="40" builtinId="44"/>
+    <cellStyle name="Accent5" xfId="41" builtinId="45"/>
+    <cellStyle name="20% - Accent5" xfId="42" builtinId="46"/>
+    <cellStyle name="40% - Accent5" xfId="43" builtinId="47"/>
+    <cellStyle name="60% - Accent5" xfId="44" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="45" builtinId="49"/>
+    <cellStyle name="20% - Accent6" xfId="46" builtinId="50"/>
     <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
     <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
@@ -1830,18 +1778,18 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:C114"/>
+  <dimension ref="A1:C104"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="125" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="A33" sqref="$A33:$XFD33"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="125" topLeftCell="A87" workbookViewId="0">
+      <selection activeCell="A100" sqref="A100"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.7013888888889" defaultRowHeight="16.2" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="10.7" defaultRowHeight="16" outlineLevelCol="2"/>
   <cols>
     <col min="1" max="1" width="26" style="1" customWidth="1"/>
-    <col min="2" max="2" width="144.1875" style="2" customWidth="1"/>
-    <col min="3" max="5" width="21.2986111111111" style="3" customWidth="1"/>
-    <col min="6" max="16384" width="10.7013888888889" style="3"/>
+    <col min="2" max="2" width="144.185714285714" style="2" customWidth="1"/>
+    <col min="3" max="5" width="21.3" style="3" customWidth="1"/>
+    <col min="6" max="16384" width="10.7" style="3"/>
   </cols>
   <sheetData>
     <row r="1" ht="23.1" customHeight="1" spans="1:2">
@@ -2555,7 +2503,7 @@
       <c r="A89" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="B89" s="2" t="s">
+      <c r="B89" t="s">
         <v>176</v>
       </c>
     </row>
@@ -2679,267 +2627,195 @@
         <v>206</v>
       </c>
     </row>
-    <row r="105" spans="1:2">
-      <c r="A105" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="B105" s="2" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="106" spans="1:2">
-      <c r="A106" s="1" t="s">
-        <v>209</v>
-      </c>
-      <c r="B106" s="2" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="107" spans="1:2">
-      <c r="A107" s="1" t="s">
-        <v>211</v>
-      </c>
-      <c r="B107" s="2" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="108" spans="1:2">
-      <c r="A108" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="B108" s="2" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="109" spans="1:2">
-      <c r="A109" s="1" t="s">
-        <v>215</v>
-      </c>
-      <c r="B109" s="2" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="110" spans="1:2">
-      <c r="A110" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="B110" s="2" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="111" spans="1:2">
-      <c r="A111" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="B111" s="2" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="112" spans="1:2">
-      <c r="A112" s="1" t="s">
-        <v>221</v>
-      </c>
-      <c r="B112" s="2" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="113" spans="1:2">
-      <c r="A113" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="B113" s="2" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="114" spans="1:2">
-      <c r="A114" s="1" t="s">
-        <v>225</v>
-      </c>
-      <c r="B114" s="2" t="s">
-        <v>226</v>
-      </c>
-    </row>
   </sheetData>
   <sheetProtection sheet="1" formatColumns="0" formatRows="0" insertRows="0" insertColumns="0" deleteColumns="0" deleteRows="0" sort="0"/>
   <conditionalFormatting sqref="A25">
-    <cfRule type="notContainsBlanks" dxfId="0" priority="20" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="0" priority="22" stopIfTrue="1">
       <formula>LEN(TRIM(A25))&gt;0</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="1" priority="19" stopIfTrue="1" operator="equal" text="nexial.">
+    <cfRule type="beginsWith" dxfId="1" priority="21" stopIfTrue="1" operator="equal" text="nexial.">
       <formula>LEFT(A25,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="2" priority="18" stopIfTrue="1" operator="equal" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="2" priority="20" stopIfTrue="1" operator="equal" text="nexial.scope.">
       <formula>LEFT(A25,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="3" priority="17" stopIfTrue="1" operator="equal" text="//">
+    <cfRule type="beginsWith" dxfId="3" priority="19" stopIfTrue="1" operator="equal" text="//">
       <formula>LEFT(A25,LEN("//"))="//"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B25">
-    <cfRule type="notContainsBlanks" dxfId="4" priority="22">
+    <cfRule type="notContainsBlanks" dxfId="4" priority="24">
       <formula>LEN(TRIM(B25))&gt;0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="5" priority="21" stopIfTrue="1">
+    <cfRule type="expression" dxfId="5" priority="23" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1),13)="nexial.scope."</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A26">
-    <cfRule type="beginsWith" dxfId="3" priority="35" stopIfTrue="1" operator="equal" text="//">
+    <cfRule type="beginsWith" dxfId="3" priority="37" stopIfTrue="1" operator="equal" text="//">
       <formula>LEFT(A26,LEN("//"))="//"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="2" priority="36" stopIfTrue="1" operator="equal" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="2" priority="38" stopIfTrue="1" operator="equal" text="nexial.scope.">
       <formula>LEFT(A26,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="1" priority="37" stopIfTrue="1" operator="equal" text="nexial.">
+    <cfRule type="beginsWith" dxfId="1" priority="39" stopIfTrue="1" operator="equal" text="nexial.">
       <formula>LEFT(A26,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="0" priority="38" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="0" priority="40" stopIfTrue="1">
       <formula>LEN(TRIM(A26))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B26">
-    <cfRule type="expression" dxfId="5" priority="39" stopIfTrue="1">
+    <cfRule type="expression" dxfId="5" priority="41" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1),13)="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="4" priority="40">
+    <cfRule type="notContainsBlanks" dxfId="4" priority="42">
       <formula>LEN(TRIM(B26))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A30">
-    <cfRule type="beginsWith" dxfId="3" priority="23" stopIfTrue="1" operator="equal" text="//">
+    <cfRule type="beginsWith" dxfId="3" priority="25" stopIfTrue="1" operator="equal" text="//">
       <formula>LEFT(A30,LEN("//"))="//"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="2" priority="24" stopIfTrue="1" operator="equal" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="2" priority="26" stopIfTrue="1" operator="equal" text="nexial.scope.">
       <formula>LEFT(A30,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="1" priority="25" stopIfTrue="1" operator="equal" text="nexial.">
+    <cfRule type="beginsWith" dxfId="1" priority="27" stopIfTrue="1" operator="equal" text="nexial.">
       <formula>LEFT(A30,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="0" priority="26" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="0" priority="28" stopIfTrue="1">
       <formula>LEN(TRIM(A30))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B30">
-    <cfRule type="expression" dxfId="5" priority="27" stopIfTrue="1">
+    <cfRule type="expression" dxfId="5" priority="29" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1),13)="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="4" priority="28">
+    <cfRule type="notContainsBlanks" dxfId="4" priority="30">
       <formula>LEN(TRIM(B30))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A50">
-    <cfRule type="beginsWith" dxfId="3" priority="1" stopIfTrue="1" operator="equal" text="//">
+    <cfRule type="beginsWith" dxfId="3" priority="3" stopIfTrue="1" operator="equal" text="//">
       <formula>LEFT(A50,LEN("//"))="//"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="2" priority="2" stopIfTrue="1" operator="equal" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="2" priority="4" stopIfTrue="1" operator="equal" text="nexial.scope.">
       <formula>LEFT(A50,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="1" priority="3" stopIfTrue="1" operator="equal" text="nexial.">
+    <cfRule type="beginsWith" dxfId="1" priority="5" stopIfTrue="1" operator="equal" text="nexial.">
       <formula>LEFT(A50,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="0" priority="4" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="0" priority="6" stopIfTrue="1">
       <formula>LEN(TRIM(A50))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B50">
-    <cfRule type="expression" dxfId="5" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="5" priority="7" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1),13)="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="4" priority="6">
+    <cfRule type="notContainsBlanks" dxfId="4" priority="8">
       <formula>LEN(TRIM(B50))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A52">
-    <cfRule type="beginsWith" dxfId="3" priority="11" stopIfTrue="1" operator="equal" text="//">
+    <cfRule type="beginsWith" dxfId="3" priority="13" stopIfTrue="1" operator="equal" text="//">
       <formula>LEFT(A52,LEN("//"))="//"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="2" priority="12" stopIfTrue="1" operator="equal" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="2" priority="14" stopIfTrue="1" operator="equal" text="nexial.scope.">
       <formula>LEFT(A52,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="1" priority="13" stopIfTrue="1" operator="equal" text="nexial.">
+    <cfRule type="beginsWith" dxfId="1" priority="15" stopIfTrue="1" operator="equal" text="nexial.">
       <formula>LEFT(A52,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="0" priority="14" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="0" priority="16" stopIfTrue="1">
       <formula>LEN(TRIM(A52))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B104">
+    <cfRule type="expression" dxfId="5" priority="1" stopIfTrue="1">
+      <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1),13)="nexial.scope."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="4" priority="2">
+      <formula>LEN(TRIM(B104))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:A3">
-    <cfRule type="beginsWith" dxfId="3" priority="41" stopIfTrue="1" operator="equal" text="//">
+    <cfRule type="beginsWith" dxfId="3" priority="43" stopIfTrue="1" operator="equal" text="//">
       <formula>LEFT(A1,LEN("//"))="//"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="2" priority="42" stopIfTrue="1" operator="equal" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="2" priority="44" stopIfTrue="1" operator="equal" text="nexial.scope.">
       <formula>LEFT(A1,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="1" priority="43" stopIfTrue="1" operator="equal" text="nexial.">
+    <cfRule type="beginsWith" dxfId="1" priority="45" stopIfTrue="1" operator="equal" text="nexial.">
       <formula>LEFT(A1,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="0" priority="44" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="0" priority="46" stopIfTrue="1">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A27:A29">
-    <cfRule type="beginsWith" dxfId="3" priority="29" stopIfTrue="1" operator="equal" text="//">
+    <cfRule type="beginsWith" dxfId="3" priority="31" stopIfTrue="1" operator="equal" text="//">
       <formula>LEFT(A27,LEN("//"))="//"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="2" priority="30" stopIfTrue="1" operator="equal" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="2" priority="32" stopIfTrue="1" operator="equal" text="nexial.scope.">
       <formula>LEFT(A27,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="1" priority="31" stopIfTrue="1" operator="equal" text="nexial.">
+    <cfRule type="beginsWith" dxfId="1" priority="33" stopIfTrue="1" operator="equal" text="nexial.">
       <formula>LEFT(A27,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="0" priority="32" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="0" priority="34" stopIfTrue="1">
       <formula>LEN(TRIM(A27))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A62:A66">
-    <cfRule type="beginsWith" dxfId="3" priority="7" stopIfTrue="1" operator="equal" text="//">
+    <cfRule type="beginsWith" dxfId="3" priority="9" stopIfTrue="1" operator="equal" text="//">
       <formula>LEFT(A62,LEN("//"))="//"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="2" priority="8" stopIfTrue="1" operator="equal" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="2" priority="10" stopIfTrue="1" operator="equal" text="nexial.scope.">
       <formula>LEFT(A62,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="1" priority="9" stopIfTrue="1" operator="equal" text="nexial.">
+    <cfRule type="beginsWith" dxfId="1" priority="11" stopIfTrue="1" operator="equal" text="nexial.">
       <formula>LEFT(A62,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="0" priority="10" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="0" priority="12" stopIfTrue="1">
       <formula>LEN(TRIM(A62))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B3">
-    <cfRule type="expression" dxfId="5" priority="45" stopIfTrue="1">
+    <cfRule type="expression" dxfId="5" priority="47" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1),13)="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="4" priority="46">
+    <cfRule type="notContainsBlanks" dxfId="4" priority="48">
       <formula>LEN(TRIM(B1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B27:B29">
-    <cfRule type="expression" dxfId="5" priority="33" stopIfTrue="1">
+    <cfRule type="expression" dxfId="5" priority="35" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1),13)="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="4" priority="34">
+    <cfRule type="notContainsBlanks" dxfId="4" priority="36">
       <formula>LEN(TRIM(B27))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C1:E3 B4:E24 C25:E32 B31:B32 B67:E84 B118:E1048576 B66 B51:B61 B33:E49 C50:E62">
-    <cfRule type="expression" dxfId="5" priority="51" stopIfTrue="1">
+  <conditionalFormatting sqref="C1:E3 B4:E24 C25:E32 B31:B32 B67:E79 B66 B51:B61 C50:E62 B33:E49 B99:E100 C101:E104 B105:E1048576 C98:E98">
+    <cfRule type="expression" dxfId="5" priority="53" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1),13)="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="4" priority="54">
+    <cfRule type="notContainsBlanks" dxfId="4" priority="56">
       <formula>LEN(TRIM(B1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A4:A24 A31:A49 A118:A1048576 A53:A61 A51 A82:A92 A67:A80">
-    <cfRule type="beginsWith" dxfId="3" priority="47" stopIfTrue="1" operator="equal" text="//">
+  <conditionalFormatting sqref="A4:A24 A31:A49 A67:A82 A53:A61 A51 A99 A105:A1048576">
+    <cfRule type="beginsWith" dxfId="3" priority="49" stopIfTrue="1" operator="equal" text="//">
       <formula>LEFT(A4,LEN("//"))="//"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="2" priority="48" stopIfTrue="1" operator="equal" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="2" priority="50" stopIfTrue="1" operator="equal" text="nexial.scope.">
       <formula>LEFT(A4,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="1" priority="49" stopIfTrue="1" operator="equal" text="nexial.">
+    <cfRule type="beginsWith" dxfId="1" priority="51" stopIfTrue="1" operator="equal" text="nexial.">
       <formula>LEFT(A4,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="0" priority="50" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="0" priority="52" stopIfTrue="1">
       <formula>LEN(TRIM(A4))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Test cases are updated asper the new updates on the GNU website elements
</commit_message>
<xml_diff>
--- a/tests/artifact/data/BalanceSheet.data.xlsx
+++ b/tests/artifact/data/BalanceSheet.data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="9215" tabRatio="500"/>
+    <workbookView windowWidth="23040" windowHeight="9024" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="#default" sheetId="2" r:id="rId1"/>
@@ -160,7 +160,7 @@
     <t>password</t>
   </si>
   <si>
-    <t>crypt:a778b096dd48a3e533c7f774e607425ec041ca57f192e5de</t>
+    <t>crypt:7c3f2ca0d17957cae090ee0ca90ea1ebd4b499130464e451</t>
   </si>
   <si>
     <t>button.submit</t>
@@ -178,7 +178,7 @@
     <t>title.header</t>
   </si>
   <si>
-    <t>//*[text()='User Login to GNUKhata']</t>
+    <t>User Login ΓÇö GNUKhata</t>
   </si>
   <si>
     <t>org.open</t>
@@ -721,12 +721,12 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="178" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="179" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="27">
     <font>
@@ -787,64 +787,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -880,31 +827,18 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -922,6 +856,72 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -932,19 +932,145 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -956,151 +1082,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1142,6 +1142,39 @@
     </border>
     <border>
       <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
@@ -1152,6 +1185,21 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1173,6 +1221,15 @@
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -1181,210 +1238,153 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="179" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="21" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="6" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1422,52 +1422,52 @@
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
-    <cellStyle name="Comma" xfId="2" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
-    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
-    <cellStyle name="Currency" xfId="5" builtinId="4"/>
-    <cellStyle name="Percent" xfId="6" builtinId="5"/>
-    <cellStyle name="Hyperlink" xfId="7" builtinId="8"/>
-    <cellStyle name="60% - Accent4" xfId="8" builtinId="44"/>
-    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9"/>
-    <cellStyle name="Check Cell" xfId="10" builtinId="23"/>
-    <cellStyle name="Heading 2" xfId="11" builtinId="17"/>
-    <cellStyle name="Note" xfId="12" builtinId="10"/>
-    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
-    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
-    <cellStyle name="Title" xfId="16" builtinId="15"/>
-    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
-    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
-    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
-    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
-    <cellStyle name="Input" xfId="21" builtinId="20"/>
-    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
-    <cellStyle name="Good" xfId="23" builtinId="26"/>
-    <cellStyle name="Output" xfId="24" builtinId="21"/>
-    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
-    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
-    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
-    <cellStyle name="Total" xfId="28" builtinId="25"/>
-    <cellStyle name="Bad" xfId="29" builtinId="27"/>
-    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
-    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
-    <cellStyle name="20% - Accent5" xfId="32" builtinId="46"/>
-    <cellStyle name="60% - Accent1" xfId="33" builtinId="32"/>
-    <cellStyle name="Accent2" xfId="34" builtinId="33"/>
-    <cellStyle name="20% - Accent2" xfId="35" builtinId="34"/>
-    <cellStyle name="20% - Accent6" xfId="36" builtinId="50"/>
-    <cellStyle name="60% - Accent2" xfId="37" builtinId="36"/>
-    <cellStyle name="Accent3" xfId="38" builtinId="37"/>
-    <cellStyle name="20% - Accent3" xfId="39" builtinId="38"/>
-    <cellStyle name="Accent4" xfId="40" builtinId="41"/>
-    <cellStyle name="20% - Accent4" xfId="41" builtinId="42"/>
-    <cellStyle name="40% - Accent4" xfId="42" builtinId="43"/>
-    <cellStyle name="Accent5" xfId="43" builtinId="45"/>
-    <cellStyle name="40% - Accent5" xfId="44" builtinId="47"/>
-    <cellStyle name="60% - Accent5" xfId="45" builtinId="48"/>
-    <cellStyle name="Accent6" xfId="46" builtinId="49"/>
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Currency" xfId="2" builtinId="4"/>
+    <cellStyle name="Percent" xfId="3" builtinId="5"/>
+    <cellStyle name="Comma [0]" xfId="4" builtinId="6"/>
+    <cellStyle name="Currency [0]" xfId="5" builtinId="7"/>
+    <cellStyle name="Hyperlink" xfId="6" builtinId="8"/>
+    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9"/>
+    <cellStyle name="Note" xfId="8" builtinId="10"/>
+    <cellStyle name="Warning Text" xfId="9" builtinId="11"/>
+    <cellStyle name="Title" xfId="10" builtinId="15"/>
+    <cellStyle name="CExplanatory Text" xfId="11" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="12" builtinId="16"/>
+    <cellStyle name="Heading 2" xfId="13" builtinId="17"/>
+    <cellStyle name="Heading 3" xfId="14" builtinId="18"/>
+    <cellStyle name="Heading 4" xfId="15" builtinId="19"/>
+    <cellStyle name="Input" xfId="16" builtinId="20"/>
+    <cellStyle name="Output" xfId="17" builtinId="21"/>
+    <cellStyle name="Calculation" xfId="18" builtinId="22"/>
+    <cellStyle name="Check Cell" xfId="19" builtinId="23"/>
+    <cellStyle name="Linked Cell" xfId="20" builtinId="24"/>
+    <cellStyle name="Total" xfId="21" builtinId="25"/>
+    <cellStyle name="Good" xfId="22" builtinId="26"/>
+    <cellStyle name="Bad" xfId="23" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="24" builtinId="28"/>
+    <cellStyle name="Accent1" xfId="25" builtinId="29"/>
+    <cellStyle name="20% - Accent1" xfId="26" builtinId="30"/>
+    <cellStyle name="40% - Accent1" xfId="27" builtinId="31"/>
+    <cellStyle name="60% - Accent1" xfId="28" builtinId="32"/>
+    <cellStyle name="Accent2" xfId="29" builtinId="33"/>
+    <cellStyle name="20% - Accent2" xfId="30" builtinId="34"/>
+    <cellStyle name="40% - Accent2" xfId="31" builtinId="35"/>
+    <cellStyle name="60% - Accent2" xfId="32" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="33" builtinId="37"/>
+    <cellStyle name="20% - Accent3" xfId="34" builtinId="38"/>
+    <cellStyle name="40% - Accent3" xfId="35" builtinId="39"/>
+    <cellStyle name="60% - Accent3" xfId="36" builtinId="40"/>
+    <cellStyle name="Accent4" xfId="37" builtinId="41"/>
+    <cellStyle name="20% - Accent4" xfId="38" builtinId="42"/>
+    <cellStyle name="40% - Accent4" xfId="39" builtinId="43"/>
+    <cellStyle name="60% - Accent4" xfId="40" builtinId="44"/>
+    <cellStyle name="Accent5" xfId="41" builtinId="45"/>
+    <cellStyle name="20% - Accent5" xfId="42" builtinId="46"/>
+    <cellStyle name="40% - Accent5" xfId="43" builtinId="47"/>
+    <cellStyle name="60% - Accent5" xfId="44" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="45" builtinId="49"/>
+    <cellStyle name="20% - Accent6" xfId="46" builtinId="50"/>
     <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
     <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
@@ -1832,8 +1832,8 @@
   <sheetPr/>
   <dimension ref="A1:C114"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="125" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="A33" sqref="$A33:$XFD33"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="125" topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="B68" sqref="B68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7013888888889" defaultRowHeight="16.2" outlineLevelCol="2"/>

</xml_diff>